<commit_message>
updated thinking and MVP
</commit_message>
<xml_diff>
--- a/Daily Project Journal_V2.xlsx
+++ b/Daily Project Journal_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EEA0F5-17EE-463F-9B05-F2EC5B42F834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF997888-4410-4F2A-BE91-D32D56F62B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="17010" windowHeight="9180" tabRatio="877" firstSheet="2" activeTab="7" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVPFeatures" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="178">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -663,6 +663,21 @@
   </si>
   <si>
     <t>Proprietary Data collection</t>
+  </si>
+  <si>
+    <t>-- Given need for ESG reporting in 2024, there will be fast, massive adoption of need to know. Pivot away from just renewable energy research. Start with collecting/summarizing data and step 1a of Decarb Strategist Process</t>
+  </si>
+  <si>
+    <t>-- 3 PERTINENT features for MVP:</t>
+  </si>
+  <si>
+    <t>--- (1) Collect reported ESG data from any company that publishes these metrics and summarizes what's used</t>
+  </si>
+  <si>
+    <t>--- (2) Sends users related, real-time updates from the web based on past queries</t>
+  </si>
+  <si>
+    <t>--- (3) Walks users through process of collecting internal data for comparison</t>
   </si>
 </sst>
 </file>
@@ -773,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -826,6 +841,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8042,10 +8063,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8064,155 +8085,191 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="10">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B8" s="16">
         <v>45122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="16">
-        <v>45122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="17"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="19"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="B11" s="16">
+        <v>45122</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-    </row>
-    <row r="17" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>84</v>
       </c>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>75</v>
-      </c>
+    <row r="22" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+    </row>
+    <row r="23" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="A24" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>72</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
         <v>77</v>
       </c>
     </row>
@@ -12100,7 +12157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27BADC2A-0533-4A25-AC3D-DC8353FFB003}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated flow for ESG
</commit_message>
<xml_diff>
--- a/Daily Project Journal_V2.xlsx
+++ b/Daily Project Journal_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFAE01E-6FB9-4E4F-B235-2D7C4FAA8F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3933E754-8AFB-4D7E-9F8D-A274218653B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37550" yWindow="110" windowWidth="20000" windowHeight="20620" tabRatio="877" activeTab="6" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="35460" yWindow="340" windowWidth="19810" windowHeight="13940" tabRatio="877" firstSheet="4" activeTab="6" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVPFeatures" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="DailyRoutineWeeklyGoal" sheetId="9" r:id="rId4"/>
     <sheet name="ActivityMap" sheetId="10" r:id="rId5"/>
     <sheet name="WorkFlow" sheetId="7" r:id="rId6"/>
-    <sheet name="QuestionsFollowUp" sheetId="8" r:id="rId7"/>
-    <sheet name="HelpfulDocumentation" sheetId="2" r:id="rId8"/>
-    <sheet name="AdditionalFeatures" sheetId="3" r:id="rId9"/>
-    <sheet name="UseCases" sheetId="4" r:id="rId10"/>
-    <sheet name="Monetization" sheetId="5" r:id="rId11"/>
+    <sheet name="ESG_WorkFlow" sheetId="12" r:id="rId7"/>
+    <sheet name="QuestionsFollowUp" sheetId="8" r:id="rId8"/>
+    <sheet name="HelpfulDocumentation" sheetId="2" r:id="rId9"/>
+    <sheet name="AdditionalFeatures" sheetId="3" r:id="rId10"/>
+    <sheet name="UseCases" sheetId="4" r:id="rId11"/>
+    <sheet name="Monetization" sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="181">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -684,6 +685,9 @@
   </si>
   <si>
     <t>What techniques work better than fine-tuning, prompt engineering, or using RAG? Better to keep to a specific knowledge domain or process?</t>
+  </si>
+  <si>
+    <t>Spoke with HongTai. Do research on market participants, tools, costs, and the product itself.</t>
   </si>
 </sst>
 </file>
@@ -794,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -848,6 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7648,6 +7653,2714 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>567652</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>144319</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Smiley Face 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04260FB8-B8AA-9AA3-AF98-4944DC71E959}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1173788" y="875531"/>
+          <a:ext cx="788940" cy="692727"/>
+        </a:xfrm>
+        <a:prstGeom prst="smileyFace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>144319</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>110643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>558030</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>125077</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CF2E66-F3DF-C089-88F8-556C1D1EFC74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1962728" y="1207461"/>
+          <a:ext cx="1625984" cy="14434"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>558030</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>481061</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>182802</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AACE33F5-BEBF-7485-7EA3-80F0FFE10827}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3588712" y="952499"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>125076</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>48106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>519545</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>134697</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9074BB-E2BC-3240-C8C3-FB499BD19AD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943485" y="1144924"/>
+          <a:ext cx="1606742" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>User Landing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Page</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>481061</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>99482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200505</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>110643</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E7E7A7-0E7E-4135-9159-53B4DCF2C0BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="21" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4117879" y="1196300"/>
+          <a:ext cx="1537853" cy="11161"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219748</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>558030</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>17703</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{531BBE6F-777C-4750-971B-E77E9D872EC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3250430" y="567652"/>
+          <a:ext cx="1550555" cy="364066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Start New?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200505</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>27323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123535</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171641</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Oval 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{412A9EF2-4CD8-41D6-89F8-605469FD5FEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5655732" y="941338"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>429876</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>48107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>163561</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>35406</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25186E22-FA8B-4223-92ED-58994E48E62D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5278967" y="596516"/>
+          <a:ext cx="1552094" cy="352905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Which framework?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123535</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>99482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9621</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C644930-F9CC-4D23-9939-9BA5C50FE89A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="21" idx="6"/>
+          <a:endCxn id="73" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6184899" y="1196300"/>
+          <a:ext cx="492222" cy="6352"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>327121</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>490682</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20614F02-A1F0-F293-D95F-11D841F374F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12449848" y="788939"/>
+          <a:ext cx="1981970" cy="846667"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Questions to answer each metric</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>490682</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>115455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>45025</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117183</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BE9163A-2908-439F-9EE5-9D4A3C376E57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="29" idx="3"/>
+          <a:endCxn id="35" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14431818" y="1212273"/>
+          <a:ext cx="766616" cy="1728"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>45025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>45024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>574192</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6539</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Oval 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99429A1C-B4B4-4D4E-8F46-E6DD7F584B02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15198434" y="959039"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>383309</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>332122</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106024</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8852FEBD-4E11-45F5-A95D-ACD2A36881B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="87" idx="3"/>
+          <a:endCxn id="97" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10687627" y="1201112"/>
+          <a:ext cx="554950" cy="1730"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>303261</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>9620</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139702</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="TextBox 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F85955E5-6D38-4141-B11B-74023C738E91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15456670" y="394470"/>
+          <a:ext cx="1524768" cy="659247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Skip Question,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>continue, save/exit?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>369070</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>25788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>102754</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>13087</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="TextBox 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E335D4-AF86-4027-A6F4-E2A15E31F9BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16128615" y="939803"/>
+          <a:ext cx="1552094" cy="352905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Continue</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>118919</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>35408</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>458741</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144318</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="TextBox 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B10260-36DE-4B55-97DF-E66EA2CE81E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6180283" y="2594650"/>
+          <a:ext cx="1552094" cy="657320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pick New Framework or Save and start new?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482793</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>309609</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>73889</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Connector: Elbow 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{864B7E3D-9723-5CCE-C514-41AB3A784285}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="4"/>
+          <a:endCxn id="50" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9844230" y="-2437247"/>
+          <a:ext cx="1712578" cy="9524998"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 113348"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>218209</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>112375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>141239</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>73889</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Oval 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF784C82-424D-43A3-A990-157D8181BC66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5673436" y="2671617"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>465089</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171641</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482793</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>112375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Straight Arrow Connector 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4752101-B9FD-12DF-C34E-F6D2E93FA7AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="0"/>
+          <a:endCxn id="21" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5920316" y="1451262"/>
+          <a:ext cx="17704" cy="1220355"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>11546</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>351367</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>78893</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="TextBox 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{108FE484-0E05-4E56-B2CF-99DECF416167}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13952682" y="3016443"/>
+          <a:ext cx="1552094" cy="352905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Save and Exit to Main</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>98138</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>134697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76969</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88515</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="TextBox 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FABE9697-21C2-49D2-96E5-CDF22BCAC423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5553365" y="2328333"/>
+          <a:ext cx="584968" cy="319424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>216478</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>182802</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>218209</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1731</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Connector: Elbow 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{283ABB06-7D87-C889-2343-8BEB049E3F28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="2"/>
+          <a:endCxn id="7" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3853296" y="1462423"/>
+          <a:ext cx="1820140" cy="1464156"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>481447</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>181263</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>460278</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>135081</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="TextBox 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F39C2E5-B8BD-448F-9422-FDFB4527CFF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4118265" y="912475"/>
+          <a:ext cx="584968" cy="319424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9621</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>134697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>586894</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76970</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Rectangle: Rounded Corners 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8F97A23-95BB-5CB1-31AA-F52ECEC64AD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6677121" y="683106"/>
+          <a:ext cx="1183409" cy="1039091"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>GRI</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>SASB</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>TFCD</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>etc.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>586894</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>516465</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>107564</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Straight Arrow Connector 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8006E24A-7ED8-4529-9FF8-444781902899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="73" idx="3"/>
+          <a:endCxn id="83" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7860530" y="1202652"/>
+          <a:ext cx="535708" cy="1730"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>516465</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>35405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>439496</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>179723</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Oval 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD364D22-3508-438D-A4FA-1068D852C164}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8396238" y="949420"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>293640</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>65810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>27325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>53109</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="TextBox 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCDB4AF9-9755-4FB2-9D0F-091843167B00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8173413" y="614219"/>
+          <a:ext cx="1552094" cy="352905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Which Section?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>412173</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133157</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>383309</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>75430</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="87" name="Rectangle: Rounded Corners 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46ABEEE7-A09B-4AAB-9B7C-FF44B92BCD1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9504218" y="681566"/>
+          <a:ext cx="1183409" cy="1039091"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Technical</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Ecocnomic</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Environmental</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Social</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>etc.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>439496</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>412173</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>107564</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="Straight Arrow Connector 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001104E1-F79E-4605-83EE-4B2622E5AD1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="83" idx="6"/>
+          <a:endCxn id="87" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8925405" y="1201112"/>
+          <a:ext cx="578813" cy="3270"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>332122</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>33865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>255153</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>178183</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Oval 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DEFA5EB-2196-4CEC-9F9C-4F0AF2CCA26A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11242577" y="947880"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>11545</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>351367</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88515</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="TextBox 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFDB13B6-8695-4903-A1B0-9768261727CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10922000" y="240530"/>
+          <a:ext cx="1552094" cy="579197"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Start with Which metric?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>255153</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>327121</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>115455</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="Straight Arrow Connector 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F83A7A15-B30F-4FC9-9875-1BA62CC9C368}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="97" idx="6"/>
+          <a:endCxn id="29" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11771744" y="1202842"/>
+          <a:ext cx="678104" cy="9431"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>574192</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>115455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>230909</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117183</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="Straight Arrow Connector 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DF60719-971B-4AC8-B580-8BB030DFC014}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="35" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15727601" y="1212273"/>
+          <a:ext cx="1475126" cy="1728"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>309610</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>144315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>211671</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>45024</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="114" name="Connector: Elbow 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71B01652-FD83-C0F7-83EA-81371B3C40F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="16007293" y="-217156"/>
+          <a:ext cx="631921" cy="1720470"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>62735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>466821</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50034</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="116" name="TextBox 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6D3867-DD5B-4A9C-B3BB-F9F4E150AE22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15886545" y="62735"/>
+          <a:ext cx="1552094" cy="352905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Skip Question</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>65809</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>594976</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>46565</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="Oval 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{209A4FA6-409C-46D0-B7E3-4C996F6D8C3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3702627" y="4289520"/>
+          <a:ext cx="529167" cy="509924"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352906</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85052</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83511</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="120" name="TextBox 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3057BA0-3FB1-4D6D-AD1A-35037AABC463}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3383588" y="3923915"/>
+          <a:ext cx="1550555" cy="364066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Compare to peers?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>594976</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>585354</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157980</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="121" name="Straight Arrow Connector 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE753497-D61D-4BA1-82DF-AF5852899177}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="119" idx="6"/>
+          <a:endCxn id="132" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4231794" y="4544482"/>
+          <a:ext cx="1808787" cy="771"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>591897</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>35405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>324043</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>33865</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="124" name="TextBox 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49D49D42-1947-496F-9F88-48F1663EDDAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4228715" y="4239875"/>
+          <a:ext cx="1550555" cy="364066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Browse industries</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>330392</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>46565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>35403</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>89092</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="Connector: Elbow 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA69FC89-8ED8-41FE-95E1-10DC4C3F618D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="119" idx="4"/>
+          <a:endCxn id="136" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4736521" y="4030133"/>
+          <a:ext cx="590936" cy="2129557"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>417177</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>149323</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>138159</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="TextBox 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6009E4F1-E29F-4927-9D8E-56AF2E40F9A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4053995" y="5075381"/>
+          <a:ext cx="1550555" cy="364066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Help me find my peers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>585354</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>8081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>556490</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>125075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="132" name="Rectangle: Rounded Corners 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB7686D1-79B5-4292-BBFB-DFE1CF9454BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6040581" y="4212551"/>
+          <a:ext cx="1183409" cy="665403"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>View database</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>35404</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>121996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>6541</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>56187</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="136" name="Rectangle: Rounded Corners 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12D4D58B-C69E-4CCE-9C90-634666362DC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096768" y="5057678"/>
+          <a:ext cx="1183409" cy="665403"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Answer questiosn</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -8305,6 +11018,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67949674-8283-46A5-8E57-0FA23CFAF458}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE19399-4494-48E4-9236-2FC54C1C696D}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -8364,7 +11107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDB856F-E16D-4194-BAE3-6CAA5BF179F2}">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -8420,13 +11163,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C65F3B7-4679-46BB-9C6C-4439D434827C}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8464,46 +11207,46 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
+        <v>45202</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="27">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>45152</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B4" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>45144</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>45143</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>33</v>
@@ -8512,10 +11255,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>45142</v>
+        <v>45143</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>33</v>
@@ -8524,7 +11267,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>45141</v>
+        <v>45142</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>125</v>
@@ -8536,34 +11279,34 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>45140</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>45139</v>
+        <v>45140</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>33</v>
@@ -8572,7 +11315,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>45138</v>
+        <v>45139</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>121</v>
@@ -8584,10 +11327,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>45137</v>
+        <v>45138</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>33</v>
@@ -8596,7 +11339,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>45136</v>
+        <v>45137</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>122</v>
@@ -8608,7 +11351,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>45135</v>
+        <v>45136</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>122</v>
@@ -8619,23 +11362,23 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="22">
+      <c r="A15" s="4">
+        <v>45135</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
         <v>45134</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B16" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>45133</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -8644,58 +11387,58 @@
     </row>
     <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>45132</v>
+        <v>45133</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>45131</v>
+        <v>45132</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>45130</v>
+        <v>45131</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>45129</v>
+        <v>45130</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>45128</v>
+        <v>45129</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
@@ -8704,118 +11447,118 @@
     </row>
     <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>45127</v>
+        <v>45128</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>45126</v>
+        <v>45127</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>45124</v>
+        <v>45125</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>45123</v>
+        <v>45124</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>45122</v>
+        <v>45123</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>45121</v>
+        <v>45122</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
+        <v>45121</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
         <v>45120</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
-        <v>45119</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="C30" t="s">
         <v>33</v>
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>45118</v>
+        <v>45119</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
@@ -8824,10 +11567,10 @@
     </row>
     <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>45117</v>
+        <v>45118</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
@@ -8836,10 +11579,10 @@
     </row>
     <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>45116</v>
+        <v>45117</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
@@ -8848,58 +11591,58 @@
     </row>
     <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>45115</v>
+        <v>45116</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
         <v>33</v>
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
+        <v>45115</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
         <v>45114</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="4">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
         <v>45113</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="4">
-        <v>45112</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <v>45111</v>
+        <v>45112</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -8908,22 +11651,22 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>45110</v>
+        <v>45111</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <v>45109</v>
+        <v>45110</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>33</v>
@@ -8932,168 +11675,169 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>45108</v>
+        <v>45109</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" t="s">
-        <v>36</v>
+        <v>70</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
+        <v>45108</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
         <v>45107</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
         <v>45106</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="4">
-        <v>45105</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="4">
-        <v>45106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
-        <v>45104</v>
+        <v>45105</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="4">
+        <v>45106</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <v>45103</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>65</v>
+        <v>45104</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>45102</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>43</v>
+        <v>45103</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>36</v>
-      </c>
-      <c r="D47" s="4">
-        <v>45110</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>45102</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>44</v>
+      <c r="B48" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C48" t="s">
         <v>36</v>
       </c>
       <c r="D48" s="4">
-        <v>45117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>45101</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>38</v>
+        <v>45102</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C49" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D49" s="4">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>45101</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="4">
+        <v>45101</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C51" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="10">
+      <c r="D51" s="9"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="10">
         <v>45101</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B52" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C52" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="4">
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="4">
         <v>45101</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="4">
-        <v>45100</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" t="s">
-        <v>33</v>
-      </c>
+      <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>45100</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>28</v>
+      <c r="B54" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C54" t="s">
         <v>33</v>
@@ -9104,7 +11848,7 @@
         <v>45100</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
@@ -9115,10 +11859,10 @@
         <v>45100</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -9126,10 +11870,10 @@
         <v>45100</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -9137,21 +11881,21 @@
         <v>45100</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
-        <v>45099</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>25</v>
+        <v>45100</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
@@ -9159,14 +11903,25 @@
         <v>45099</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="61" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4">
+        <v>45099</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:D1048576 G49:G52">
+  <conditionalFormatting sqref="C1:D1048576 G50:G53">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
@@ -9416,10 +12171,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -9438,10 +12193,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="28"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -10761,7 +13516,7 @@
   <dimension ref="A1:Z71"/>
   <sheetViews>
     <sheetView zoomScale="68" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12764,10 +15519,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A35583E-4C87-49DF-851E-06955158F6FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1C4AE-2FEE-4632-8340-936389828A23}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -12802,11 +15572,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27BADC2A-0533-4A25-AC3D-DC8353FFB003}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -12836,34 +15606,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67949674-8283-46A5-8E57-0FA23CFAF458}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated deck and financials
</commit_message>
<xml_diff>
--- a/Daily Project Journal_V2.xlsx
+++ b/Daily Project Journal_V2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C240E6-DC5B-4A97-AD41-40B4F3B00183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2FCF7C-A13D-4173-829E-54F59FB8F76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="2" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="1" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualESG" sheetId="14" r:id="rId1"/>
     <sheet name="MVPFeatures" sheetId="1" r:id="rId2"/>
-    <sheet name="Personell" sheetId="15" r:id="rId3"/>
+    <sheet name="Costs" sheetId="15" r:id="rId3"/>
     <sheet name="DailyNotes" sheetId="6" r:id="rId4"/>
     <sheet name="Sources" sheetId="11" r:id="rId5"/>
     <sheet name="DailyRoutineWeeklyGoal" sheetId="9" r:id="rId6"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="313">
   <si>
     <t>List of capabilities</t>
   </si>
@@ -891,21 +891,9 @@
     <t xml:space="preserve">https://www.workiva.com/solutions/esg-reporting?utm_medium=Search&amp;utm_type=Paid&amp;utm_source=Google&amp;utm_campaign=ESG-Solutions_2022_Q2&amp;utm_solution=ESG&amp;utm_geo=North-America&amp;utm_segment=ESG-General&amp;gclid=CjwKCAjwkNOpBhBEEiwAb3MvvdcjCRKMQsbHF_QIBM9bKKhImYbQ8zOeMYQuAPSXCb8hyXPgBTZukBoCJrkQAvD_BwE </t>
   </si>
   <si>
-    <t>--- (3a) Points user to where to find relevant external data OR pulls in automatically.</t>
-  </si>
-  <si>
     <t>--- (1) Collect reported ESG data from any company that publishes these metrics and summarizes what's used, how calculated. Calculates averages and benchmarks and helps you compare your data to industry, peers.</t>
   </si>
   <si>
-    <t>--- (2) Sends users related, real-time updates from the web based on metrics and geographies of interest. (regulations, announcements, funding, relevant news, federa/state/local government regulations)</t>
-  </si>
-  <si>
-    <t>--- (3) Walks users through process of collecting internal and external data for calculations.</t>
-  </si>
-  <si>
-    <t>--- (4) Creates stunning visuals to tell the story</t>
-  </si>
-  <si>
     <t>IDEAL CUSTOMER: Any business, small to large, who is has to create an annual ESG report. They need this to get through the very first step in ESG reporting and saves them a tremendous amount of time.</t>
   </si>
   <si>
@@ -945,12 +933,6 @@
     <t>Annual Revenue:</t>
   </si>
   <si>
-    <t>publicly traded companies</t>
-  </si>
-  <si>
-    <t>100-500 people private companies</t>
-  </si>
-  <si>
     <t>Market Share [%]</t>
   </si>
   <si>
@@ -1023,28 +1005,88 @@
     <t>HR:</t>
   </si>
   <si>
-    <t>Non-Wages</t>
-  </si>
-  <si>
     <t>Computers</t>
   </si>
   <si>
-    <t>Cloud</t>
-  </si>
-  <si>
     <t>Office Rent</t>
   </si>
   <si>
     <t>Office furniture</t>
   </si>
   <si>
-    <t>Back-end Subscriptions</t>
-  </si>
-  <si>
-    <t>Front-end Subscriptions</t>
-  </si>
-  <si>
     <t>ESG Specialist</t>
+  </si>
+  <si>
+    <t>Office and Infrastructure</t>
+  </si>
+  <si>
+    <t>Cloud &amp; Database</t>
+  </si>
+  <si>
+    <t>Data scraping</t>
+  </si>
+  <si>
+    <t>Front end software</t>
+  </si>
+  <si>
+    <t>Legal/Administrative services</t>
+  </si>
+  <si>
+    <t>Total Non-Salary Costs</t>
+  </si>
+  <si>
+    <t>publicly traded companies [No]:</t>
+  </si>
+  <si>
+    <t>100-500 people private companies [No]</t>
+  </si>
+  <si>
+    <t>CAGR</t>
+  </si>
+  <si>
+    <t>Before Tax Profit</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
+  </si>
+  <si>
+    <t>Explosive Growth</t>
+  </si>
+  <si>
+    <t>Sr. Dev.</t>
+  </si>
+  <si>
+    <t>Support 3</t>
+  </si>
+  <si>
+    <t>Support 4</t>
+  </si>
+  <si>
+    <t>Total Costs (Capex and Opex)</t>
+  </si>
+  <si>
+    <t>--- (2) Walks users through process of collecting internal and external data for calculations.</t>
+  </si>
+  <si>
+    <t>--- (2a) Points user to where to find relevant external data OR pulls in automatically (for easier to obtain/calculate data)</t>
+  </si>
+  <si>
+    <t>--- (3) Creates stunning visuals to tell the story</t>
+  </si>
+  <si>
+    <t>--- (4) Sends users related, real-time updates from the web based on metrics and geographies of interest. (regulations, announcements, funding, relevant news, federa/state/local government regulations)</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1096,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -1148,13 +1190,13 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1162,7 +1204,15 @@
     <font>
       <b/>
       <u/>
-      <sz val="8"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1170,15 +1220,7 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1226,7 +1268,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1296,28 +1338,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -13355,8 +13404,8 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13391,37 +13440,37 @@
     </row>
     <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>249</v>
+        <v>309</v>
       </c>
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>250</v>
+        <v>310</v>
       </c>
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B9" s="9"/>
     </row>
@@ -13597,848 +13646,1809 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8991098-D6BF-4772-AB0B-B5195386BBAD}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:G35"/>
+    <sheetView topLeftCell="B1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="25.90625" style="35" customWidth="1"/>
+    <col min="2" max="12" width="15.6328125" style="35"/>
+    <col min="13" max="13" width="3.08984375" style="35" customWidth="1"/>
+    <col min="14" max="14" width="15.6328125" style="35"/>
+    <col min="15" max="15" width="21.453125" style="35" customWidth="1"/>
+    <col min="16" max="16384" width="15.6328125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="38">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="39" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C2" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D2" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E2" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F2" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="P2" s="40">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="39" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40">
+        <v>100</v>
+      </c>
+      <c r="D3" s="40">
+        <f>C3*1.5</f>
+        <v>150</v>
+      </c>
+      <c r="E3" s="40">
+        <f t="shared" ref="E3:G3" si="0">D3*1.5</f>
+        <v>225</v>
+      </c>
+      <c r="F3" s="40">
+        <f t="shared" si="0"/>
+        <v>337.5</v>
+      </c>
+      <c r="G3" s="40">
+        <f t="shared" si="0"/>
+        <v>506.25</v>
+      </c>
+      <c r="H3" s="40">
+        <f>G3*2</f>
+        <v>1012.5</v>
+      </c>
+      <c r="I3" s="40">
+        <f t="shared" ref="I3:L3" si="1">H3*2</f>
+        <v>2025</v>
+      </c>
+      <c r="J3" s="40">
+        <f t="shared" si="1"/>
+        <v>4050</v>
+      </c>
+      <c r="K3" s="40">
+        <f t="shared" si="1"/>
+        <v>8100</v>
+      </c>
+      <c r="L3" s="40">
+        <f t="shared" si="1"/>
+        <v>16200</v>
+      </c>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41">
+        <f>(L3/C3)^(1/COUNT(C3:L3))-1</f>
+        <v>0.66322690407688611</v>
+      </c>
+      <c r="O3" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="P3" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43">
+        <v>1200</v>
+      </c>
+      <c r="D4" s="43">
+        <v>1800</v>
+      </c>
+      <c r="E4" s="43">
+        <v>1800</v>
+      </c>
+      <c r="F4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="G4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="H4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="I4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="J4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="K4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="L4" s="43">
+        <v>2400</v>
+      </c>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="P4" s="38">
+        <f>P3*SUM(P1:P2)</f>
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38">
+        <v>2</v>
+      </c>
+      <c r="D5" s="38">
+        <v>2</v>
+      </c>
+      <c r="E5" s="38">
+        <v>2</v>
+      </c>
+      <c r="F5" s="38">
+        <v>2</v>
+      </c>
+      <c r="G5" s="38">
+        <v>2</v>
+      </c>
+      <c r="H5" s="38">
+        <v>2</v>
+      </c>
+      <c r="I5" s="38">
+        <v>2</v>
+      </c>
+      <c r="J5" s="38">
+        <v>2</v>
+      </c>
+      <c r="K5" s="38">
+        <v>2</v>
+      </c>
+      <c r="L5" s="38">
+        <v>2</v>
+      </c>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43">
+        <f t="shared" ref="C6:G6" si="2">C3*C4*C5</f>
+        <v>240000</v>
+      </c>
+      <c r="D6" s="43">
+        <f t="shared" si="2"/>
+        <v>540000</v>
+      </c>
+      <c r="E6" s="43">
+        <f t="shared" si="2"/>
+        <v>810000</v>
+      </c>
+      <c r="F6" s="43">
+        <f t="shared" si="2"/>
+        <v>1620000</v>
+      </c>
+      <c r="G6" s="43">
+        <f t="shared" si="2"/>
+        <v>2430000</v>
+      </c>
+      <c r="H6" s="43">
+        <f t="shared" ref="H6:L6" si="3">H3*H4*H5</f>
+        <v>4860000</v>
+      </c>
+      <c r="I6" s="43">
+        <f t="shared" si="3"/>
+        <v>9720000</v>
+      </c>
+      <c r="J6" s="43">
+        <f t="shared" si="3"/>
+        <v>19440000</v>
+      </c>
+      <c r="K6" s="43">
+        <f t="shared" si="3"/>
+        <v>38880000</v>
+      </c>
+      <c r="L6" s="43">
+        <f t="shared" si="3"/>
+        <v>77760000</v>
+      </c>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10" s="43">
+        <v>200000</v>
+      </c>
+      <c r="C10" s="43">
+        <v>200000</v>
+      </c>
+      <c r="D10" s="43">
+        <v>200000</v>
+      </c>
+      <c r="E10" s="43">
+        <v>200000</v>
+      </c>
+      <c r="F10" s="43">
+        <v>400000</v>
+      </c>
+      <c r="G10" s="43">
+        <v>500000</v>
+      </c>
+      <c r="H10" s="43">
+        <v>500000</v>
+      </c>
+      <c r="I10" s="43">
+        <v>500000</v>
+      </c>
+      <c r="J10" s="43">
+        <v>500000</v>
+      </c>
+      <c r="K10" s="43">
+        <v>500000</v>
+      </c>
+      <c r="L10" s="43">
+        <v>500000</v>
+      </c>
+      <c r="M10" s="43"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="43">
+        <v>150000</v>
+      </c>
+      <c r="C11" s="43">
+        <v>150000</v>
+      </c>
+      <c r="D11" s="43">
+        <v>150000</v>
+      </c>
+      <c r="E11" s="43">
+        <v>150000</v>
+      </c>
+      <c r="F11" s="43">
+        <v>300000</v>
+      </c>
+      <c r="G11" s="43">
+        <v>400000</v>
+      </c>
+      <c r="H11" s="43">
+        <v>400000</v>
+      </c>
+      <c r="I11" s="43">
+        <v>400000</v>
+      </c>
+      <c r="J11" s="43">
+        <v>400000</v>
+      </c>
+      <c r="K11" s="43">
+        <v>400000</v>
+      </c>
+      <c r="L11" s="43">
+        <v>400000</v>
+      </c>
+      <c r="M11" s="43"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" s="43">
+        <v>100000</v>
+      </c>
+      <c r="C12" s="43">
+        <v>100000</v>
+      </c>
+      <c r="D12" s="43">
+        <v>100000</v>
+      </c>
+      <c r="E12" s="43">
+        <v>100000</v>
+      </c>
+      <c r="F12" s="43">
+        <v>200000</v>
+      </c>
+      <c r="G12" s="43">
+        <v>300000</v>
+      </c>
+      <c r="H12" s="43">
+        <v>300000</v>
+      </c>
+      <c r="I12" s="43">
+        <v>300000</v>
+      </c>
+      <c r="J12" s="43">
+        <v>300000</v>
+      </c>
+      <c r="K12" s="43">
+        <v>300000</v>
+      </c>
+      <c r="L12" s="43">
+        <v>300000</v>
+      </c>
+      <c r="M12" s="43"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
         <v>272</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="42" t="s">
-        <v>265</v>
-      </c>
-      <c r="J1" s="40">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="37" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>262</v>
-      </c>
-      <c r="G2" s="37" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="B14" s="43">
+        <v>100000</v>
+      </c>
+      <c r="C14" s="43">
+        <v>100000</v>
+      </c>
+      <c r="D14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="E14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="F14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="G14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="H14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="I14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="J14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="K14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="L14" s="43">
+        <v>130000</v>
+      </c>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="I2" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="J2" s="38">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="37" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="B3" s="38">
-        <v>500</v>
-      </c>
-      <c r="C3" s="38">
-        <f>B3*2</f>
-        <v>1000</v>
-      </c>
-      <c r="D3" s="38">
-        <f t="shared" ref="D3:F3" si="0">C3*2</f>
-        <v>2000</v>
-      </c>
-      <c r="E3" s="38">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="F3" s="38">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="G3" s="38">
-        <f t="shared" ref="G3" si="1">F3*2</f>
-        <v>16000</v>
-      </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="J3" s="41">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
-        <v>270</v>
-      </c>
-      <c r="B4" s="39">
-        <v>1200</v>
-      </c>
-      <c r="C4" s="39">
-        <v>1200</v>
-      </c>
-      <c r="D4" s="39">
-        <v>1800</v>
-      </c>
-      <c r="E4" s="39">
-        <v>1800</v>
-      </c>
-      <c r="F4" s="39">
-        <v>2400</v>
-      </c>
-      <c r="G4" s="39">
-        <v>2400</v>
-      </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="36" t="s">
-        <v>268</v>
-      </c>
-      <c r="J4" s="40">
-        <f>J3*SUM(J1:J2)</f>
-        <v>12600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="B5" s="40">
-        <v>2</v>
-      </c>
-      <c r="C5" s="40">
-        <v>2</v>
-      </c>
-      <c r="D5" s="40">
-        <v>2</v>
-      </c>
-      <c r="E5" s="40">
-        <v>2</v>
-      </c>
-      <c r="F5" s="40">
-        <v>2</v>
-      </c>
-      <c r="G5" s="40">
-        <v>2</v>
-      </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="36"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
-        <v>264</v>
-      </c>
-      <c r="B6" s="39">
-        <f>B3*B4*B5</f>
-        <v>1200000</v>
-      </c>
-      <c r="C6" s="39">
-        <f t="shared" ref="C6:G6" si="2">C3*C4*C5</f>
-        <v>2400000</v>
-      </c>
-      <c r="D6" s="39">
-        <f t="shared" si="2"/>
-        <v>7200000</v>
-      </c>
-      <c r="E6" s="39">
-        <f t="shared" si="2"/>
-        <v>14400000</v>
-      </c>
-      <c r="F6" s="39">
-        <f t="shared" si="2"/>
-        <v>38400000</v>
-      </c>
-      <c r="G6" s="39">
-        <f t="shared" si="2"/>
-        <v>76800000</v>
-      </c>
-      <c r="H6" s="39"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="45" t="s">
+      <c r="B15" s="43">
+        <v>200000</v>
+      </c>
+      <c r="C15" s="43">
+        <v>200000</v>
+      </c>
+      <c r="D15" s="43">
+        <v>200000</v>
+      </c>
+      <c r="E15" s="43">
+        <v>250000</v>
+      </c>
+      <c r="F15" s="43">
+        <v>250000</v>
+      </c>
+      <c r="G15" s="43">
+        <v>250000</v>
+      </c>
+      <c r="H15" s="43">
+        <v>300000</v>
+      </c>
+      <c r="I15" s="43">
+        <v>300000</v>
+      </c>
+      <c r="J15" s="43">
+        <v>300000</v>
+      </c>
+      <c r="K15" s="43">
+        <v>300000</v>
+      </c>
+      <c r="L15" s="43">
+        <v>300000</v>
+      </c>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43">
+        <v>200000</v>
+      </c>
+      <c r="D16" s="43">
+        <v>200000</v>
+      </c>
+      <c r="E16" s="43">
+        <v>250000</v>
+      </c>
+      <c r="F16" s="43">
+        <v>250000</v>
+      </c>
+      <c r="G16" s="43">
+        <v>250000</v>
+      </c>
+      <c r="H16" s="43">
+        <v>300000</v>
+      </c>
+      <c r="I16" s="43">
+        <v>300000</v>
+      </c>
+      <c r="J16" s="43">
+        <v>300000</v>
+      </c>
+      <c r="K16" s="43">
+        <v>300000</v>
+      </c>
+      <c r="L16" s="43">
+        <v>300000</v>
+      </c>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="B17" s="43">
+        <v>130000</v>
+      </c>
+      <c r="C17" s="43">
+        <v>130000</v>
+      </c>
+      <c r="D17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="E17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="F17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="G17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="H17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="I17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="J17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="K17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="L17" s="43">
+        <v>150000</v>
+      </c>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43">
+        <v>130000</v>
+      </c>
+      <c r="D18" s="43">
+        <v>130000</v>
+      </c>
+      <c r="E18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="F18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="G18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="H18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="I18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="J18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="K18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="L18" s="43">
+        <v>150000</v>
+      </c>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43">
+        <v>250000</v>
+      </c>
+      <c r="F19" s="43">
+        <v>250000</v>
+      </c>
+      <c r="G19" s="43">
+        <v>250000</v>
+      </c>
+      <c r="H19" s="43">
+        <v>300000</v>
+      </c>
+      <c r="I19" s="43">
+        <v>300000</v>
+      </c>
+      <c r="J19" s="43">
+        <v>300000</v>
+      </c>
+      <c r="K19" s="43">
+        <v>300000</v>
+      </c>
+      <c r="L19" s="43">
+        <v>300000</v>
+      </c>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43">
+        <v>250000</v>
+      </c>
+      <c r="F20" s="43">
+        <v>250000</v>
+      </c>
+      <c r="G20" s="43">
+        <v>250000</v>
+      </c>
+      <c r="H20" s="43">
+        <v>300000</v>
+      </c>
+      <c r="I20" s="43">
+        <v>300000</v>
+      </c>
+      <c r="J20" s="43">
+        <v>300000</v>
+      </c>
+      <c r="K20" s="43">
+        <v>300000</v>
+      </c>
+      <c r="L20" s="43">
+        <v>300000</v>
+      </c>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="F21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="G21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="H21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="I21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="J21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="K21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="L21" s="43">
+        <v>150000</v>
+      </c>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="F22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="G22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="H22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="I22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="J22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="K22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="L22" s="43">
+        <v>150000</v>
+      </c>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="43">
+        <v>200000</v>
+      </c>
+      <c r="C24" s="43">
+        <v>200000</v>
+      </c>
+      <c r="D24" s="43">
+        <v>200000</v>
+      </c>
+      <c r="E24" s="43">
+        <v>200000</v>
+      </c>
+      <c r="F24" s="43">
+        <v>200000</v>
+      </c>
+      <c r="G24" s="43">
+        <v>200000</v>
+      </c>
+      <c r="H24" s="43">
+        <v>300000</v>
+      </c>
+      <c r="I24" s="43">
+        <v>300000</v>
+      </c>
+      <c r="J24" s="43">
+        <v>300000</v>
+      </c>
+      <c r="K24" s="43">
+        <v>300000</v>
+      </c>
+      <c r="L24" s="43">
+        <v>300000</v>
+      </c>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="E25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="F25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="G25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="H25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="I25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="J25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="K25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="L25" s="43">
+        <v>100000</v>
+      </c>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="E26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="F26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="G26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="H26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="I26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="J26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="K26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="L26" s="43">
+        <v>100000</v>
+      </c>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43">
+        <v>100000</v>
+      </c>
+      <c r="H27" s="43">
+        <v>100000</v>
+      </c>
+      <c r="I27" s="43">
+        <v>100000</v>
+      </c>
+      <c r="J27" s="43">
+        <v>100000</v>
+      </c>
+      <c r="K27" s="43">
+        <v>100000</v>
+      </c>
+      <c r="L27" s="43">
+        <v>100000</v>
+      </c>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43">
+        <v>100000</v>
+      </c>
+      <c r="H28" s="43">
+        <v>100000</v>
+      </c>
+      <c r="I28" s="43">
+        <v>100000</v>
+      </c>
+      <c r="J28" s="43">
+        <v>100000</v>
+      </c>
+      <c r="K28" s="43">
+        <v>100000</v>
+      </c>
+      <c r="L28" s="43">
+        <v>100000</v>
+      </c>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="35" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
-        <v>274</v>
-      </c>
-      <c r="B10" s="39">
+      <c r="B30" s="43">
+        <v>100000</v>
+      </c>
+      <c r="C30" s="43">
+        <v>100000</v>
+      </c>
+      <c r="D30" s="43">
+        <v>100000</v>
+      </c>
+      <c r="E30" s="43">
+        <v>100000</v>
+      </c>
+      <c r="F30" s="43">
+        <v>100000</v>
+      </c>
+      <c r="G30" s="43">
         <v>200000</v>
       </c>
-      <c r="C10" s="39">
+      <c r="H30" s="43">
         <v>200000</v>
       </c>
-      <c r="D10" s="39">
-        <v>400000</v>
-      </c>
-      <c r="E10" s="39">
-        <v>400000</v>
-      </c>
-      <c r="F10" s="39">
-        <v>400000</v>
-      </c>
-      <c r="G10" s="39">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
-        <v>275</v>
-      </c>
-      <c r="B11" s="39">
-        <v>150000</v>
-      </c>
-      <c r="C11" s="39">
-        <v>150000</v>
-      </c>
-      <c r="D11" s="39">
-        <v>300000</v>
-      </c>
-      <c r="E11" s="39">
-        <v>300000</v>
-      </c>
-      <c r="F11" s="39">
-        <v>300000</v>
-      </c>
-      <c r="G11" s="39">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="I30" s="43">
+        <v>200000</v>
+      </c>
+      <c r="J30" s="43">
+        <v>200000</v>
+      </c>
+      <c r="K30" s="43">
+        <v>200000</v>
+      </c>
+      <c r="L30" s="43">
+        <v>200000</v>
+      </c>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="D31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="E31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="F31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="G31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="H31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="I31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="J31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="K31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="L31" s="43">
+        <v>80000</v>
+      </c>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="E32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="F32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="G32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="H32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="I32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="J32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="K32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="L32" s="43">
+        <v>80000</v>
+      </c>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43">
+        <v>80000</v>
+      </c>
+      <c r="H33" s="43">
+        <v>80000</v>
+      </c>
+      <c r="I33" s="43">
+        <v>80000</v>
+      </c>
+      <c r="J33" s="43">
+        <v>80000</v>
+      </c>
+      <c r="K33" s="43">
+        <v>80000</v>
+      </c>
+      <c r="L33" s="43">
+        <v>80000</v>
+      </c>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43">
+        <v>80000</v>
+      </c>
+      <c r="H34" s="43">
+        <v>80000</v>
+      </c>
+      <c r="I34" s="43">
+        <v>80000</v>
+      </c>
+      <c r="J34" s="43">
+        <v>80000</v>
+      </c>
+      <c r="K34" s="43">
+        <v>80000</v>
+      </c>
+      <c r="L34" s="43">
+        <v>80000</v>
+      </c>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43">
         <v>100000</v>
       </c>
-      <c r="C12" s="39">
+      <c r="D36" s="43">
         <v>100000</v>
       </c>
-      <c r="D12" s="39">
-        <v>200000</v>
-      </c>
-      <c r="E12" s="39">
-        <v>200000</v>
-      </c>
-      <c r="F12" s="39">
-        <v>200000</v>
-      </c>
-      <c r="G12" s="39">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+      <c r="E36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="F36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="G36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="H36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="I36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="J36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="K36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="L36" s="43">
+        <v>100000</v>
+      </c>
+      <c r="M36" s="43"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="B37" s="43"/>
+      <c r="C37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="D37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="E37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="F37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="G37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="H37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="I37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="J37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="K37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="L37" s="43">
+        <v>80000</v>
+      </c>
+      <c r="M37" s="43"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="E38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="F38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="G38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="H38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="I38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="J38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="K38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="L38" s="43">
+        <v>80000</v>
+      </c>
+      <c r="M38" s="43"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="D40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="E40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="F40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="G40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="H40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="I40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="J40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="K40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="L40" s="43">
+        <v>130000</v>
+      </c>
+      <c r="M40" s="43"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="45"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+    </row>
+    <row r="43" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="46" t="s">
+        <v>283</v>
+      </c>
+      <c r="B43" s="47">
+        <f>SUM(B10:B40)</f>
+        <v>1180000</v>
+      </c>
+      <c r="C43" s="47">
+        <f t="shared" ref="C43:L43" si="4">SUM(C10:C40)</f>
+        <v>1900000</v>
+      </c>
+      <c r="D43" s="47">
+        <f t="shared" si="4"/>
+        <v>2310000</v>
+      </c>
+      <c r="E43" s="47">
+        <f t="shared" si="4"/>
+        <v>3230000</v>
+      </c>
+      <c r="F43" s="47">
+        <f t="shared" si="4"/>
+        <v>3680000</v>
+      </c>
+      <c r="G43" s="47">
+        <f t="shared" si="4"/>
+        <v>4440000</v>
+      </c>
+      <c r="H43" s="47">
+        <f t="shared" si="4"/>
+        <v>4740000</v>
+      </c>
+      <c r="I43" s="47">
+        <f t="shared" si="4"/>
+        <v>4740000</v>
+      </c>
+      <c r="J43" s="47">
+        <f t="shared" si="4"/>
+        <v>4740000</v>
+      </c>
+      <c r="K43" s="47">
+        <f t="shared" si="4"/>
+        <v>4740000</v>
+      </c>
+      <c r="L43" s="47">
+        <f t="shared" si="4"/>
+        <v>4740000</v>
+      </c>
+      <c r="M43" s="47"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="45" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="B46" s="43">
+        <f>12000*12</f>
+        <v>144000</v>
+      </c>
+      <c r="C46" s="43">
+        <f t="shared" ref="C46:G46" si="5">12000*12</f>
+        <v>144000</v>
+      </c>
+      <c r="D46" s="43">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="E46" s="43">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="F46" s="43">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="G46" s="43">
+        <f t="shared" si="5"/>
+        <v>144000</v>
+      </c>
+      <c r="H46" s="43">
+        <f>24000*12</f>
+        <v>288000</v>
+      </c>
+      <c r="I46" s="43">
+        <f t="shared" ref="I46:L46" si="6">24000*12</f>
+        <v>288000</v>
+      </c>
+      <c r="J46" s="43">
+        <f t="shared" si="6"/>
+        <v>288000</v>
+      </c>
+      <c r="K46" s="43">
+        <f t="shared" si="6"/>
+        <v>288000</v>
+      </c>
+      <c r="L46" s="43">
+        <f t="shared" si="6"/>
+        <v>288000</v>
+      </c>
+      <c r="M46" s="43"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="B47" s="43">
+        <v>30000</v>
+      </c>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43">
+        <v>30000</v>
+      </c>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43">
+        <v>50000</v>
+      </c>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" s="43">
+        <v>10000</v>
+      </c>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43">
+        <v>10000</v>
+      </c>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43">
+        <v>30000</v>
+      </c>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="B49" s="43">
+        <v>12000</v>
+      </c>
+      <c r="C49" s="43">
+        <v>12000</v>
+      </c>
+      <c r="D49" s="43">
+        <v>24000</v>
+      </c>
+      <c r="E49" s="43">
+        <v>24000</v>
+      </c>
+      <c r="F49" s="43">
+        <v>24000</v>
+      </c>
+      <c r="G49" s="43">
+        <v>24000</v>
+      </c>
+      <c r="H49" s="43">
+        <v>48000</v>
+      </c>
+      <c r="I49" s="43">
+        <v>48000</v>
+      </c>
+      <c r="J49" s="43">
+        <v>48000</v>
+      </c>
+      <c r="K49" s="43">
+        <v>48000</v>
+      </c>
+      <c r="L49" s="43">
+        <v>48000</v>
+      </c>
+      <c r="M49" s="43"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="B50" s="43">
+        <v>12000</v>
+      </c>
+      <c r="C50" s="43">
+        <v>12000</v>
+      </c>
+      <c r="D50" s="43">
+        <v>24000</v>
+      </c>
+      <c r="E50" s="43">
+        <v>24000</v>
+      </c>
+      <c r="F50" s="43">
+        <v>24000</v>
+      </c>
+      <c r="G50" s="43">
+        <v>24000</v>
+      </c>
+      <c r="H50" s="43">
+        <v>48000</v>
+      </c>
+      <c r="I50" s="43">
+        <v>48000</v>
+      </c>
+      <c r="J50" s="43">
+        <v>48000</v>
+      </c>
+      <c r="K50" s="43">
+        <v>48000</v>
+      </c>
+      <c r="L50" s="43">
+        <v>48000</v>
+      </c>
+      <c r="M50" s="43"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B51" s="43">
+        <v>12000</v>
+      </c>
+      <c r="C51" s="43">
+        <v>12000</v>
+      </c>
+      <c r="D51" s="43">
+        <v>24000</v>
+      </c>
+      <c r="E51" s="43">
+        <v>24000</v>
+      </c>
+      <c r="F51" s="43">
+        <v>24000</v>
+      </c>
+      <c r="G51" s="43">
+        <v>24000</v>
+      </c>
+      <c r="H51" s="43">
+        <v>48000</v>
+      </c>
+      <c r="I51" s="43">
+        <v>48000</v>
+      </c>
+      <c r="J51" s="43">
+        <v>48000</v>
+      </c>
+      <c r="K51" s="43">
+        <v>48000</v>
+      </c>
+      <c r="L51" s="43">
+        <v>48000</v>
+      </c>
+      <c r="M51" s="43"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="B52" s="43">
+        <v>12000</v>
+      </c>
+      <c r="C52" s="43">
+        <v>12000</v>
+      </c>
+      <c r="D52" s="43">
+        <v>24000</v>
+      </c>
+      <c r="E52" s="43">
+        <v>24000</v>
+      </c>
+      <c r="F52" s="43">
+        <v>24000</v>
+      </c>
+      <c r="G52" s="43">
+        <v>24000</v>
+      </c>
+      <c r="H52" s="43">
+        <v>48000</v>
+      </c>
+      <c r="I52" s="43">
+        <v>48000</v>
+      </c>
+      <c r="J52" s="43">
+        <v>48000</v>
+      </c>
+      <c r="K52" s="43">
+        <v>48000</v>
+      </c>
+      <c r="L52" s="43">
+        <v>48000</v>
+      </c>
+      <c r="M52" s="43"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="B54" s="48">
+        <f>SUM(B46:B52)</f>
+        <v>232000</v>
+      </c>
+      <c r="C54" s="48">
+        <f t="shared" ref="C54:L54" si="7">SUM(C46:C52)</f>
+        <v>192000</v>
+      </c>
+      <c r="D54" s="48">
+        <f t="shared" si="7"/>
+        <v>280000</v>
+      </c>
+      <c r="E54" s="48">
+        <f t="shared" si="7"/>
+        <v>240000</v>
+      </c>
+      <c r="F54" s="48">
+        <f t="shared" si="7"/>
+        <v>270000</v>
+      </c>
+      <c r="G54" s="48">
+        <f t="shared" si="7"/>
+        <v>240000</v>
+      </c>
+      <c r="H54" s="48">
+        <f t="shared" si="7"/>
+        <v>530000</v>
+      </c>
+      <c r="I54" s="48">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="J54" s="48">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="K54" s="48">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="L54" s="48">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="M54" s="48"/>
+    </row>
+    <row r="56" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="B56" s="47">
+        <f>SUM(B43,B54)</f>
+        <v>1412000</v>
+      </c>
+      <c r="C56" s="47">
+        <f t="shared" ref="C56:G56" si="8">SUM(C43,C54)</f>
+        <v>2092000</v>
+      </c>
+      <c r="D56" s="47">
+        <f t="shared" si="8"/>
+        <v>2590000</v>
+      </c>
+      <c r="E56" s="47">
+        <f t="shared" si="8"/>
+        <v>3470000</v>
+      </c>
+      <c r="F56" s="47">
+        <f t="shared" si="8"/>
+        <v>3950000</v>
+      </c>
+      <c r="G56" s="47">
+        <f t="shared" si="8"/>
+        <v>4680000</v>
+      </c>
+      <c r="H56" s="47">
+        <f t="shared" ref="H56:L56" si="9">SUM(H43,H54)</f>
+        <v>5270000</v>
+      </c>
+      <c r="I56" s="47">
+        <f t="shared" si="9"/>
+        <v>5220000</v>
+      </c>
+      <c r="J56" s="47">
+        <f t="shared" si="9"/>
+        <v>5220000</v>
+      </c>
+      <c r="K56" s="47">
+        <f t="shared" si="9"/>
+        <v>5220000</v>
+      </c>
+      <c r="L56" s="47">
+        <f t="shared" si="9"/>
+        <v>5220000</v>
+      </c>
+      <c r="M56" s="47"/>
+    </row>
+    <row r="57" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="46" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="39">
-        <v>150000</v>
-      </c>
-      <c r="C14" s="39">
-        <v>150000</v>
-      </c>
-      <c r="D14" s="39">
-        <v>150000</v>
-      </c>
-      <c r="E14" s="39">
-        <v>150000</v>
-      </c>
-      <c r="F14" s="39">
-        <v>150000</v>
-      </c>
-      <c r="G14" s="39">
-        <v>150000</v>
-      </c>
-      <c r="H14" s="39"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
-        <v>279</v>
-      </c>
-      <c r="B15" s="39">
-        <v>200000</v>
-      </c>
-      <c r="C15" s="39">
-        <v>200000</v>
-      </c>
-      <c r="D15" s="39">
-        <v>200000</v>
-      </c>
-      <c r="E15" s="39">
-        <v>250000</v>
-      </c>
-      <c r="F15" s="39">
-        <v>250000</v>
-      </c>
-      <c r="G15" s="39">
-        <v>250000</v>
-      </c>
-      <c r="H15" s="39"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
-        <v>279</v>
-      </c>
-      <c r="B16" s="39">
-        <v>200000</v>
-      </c>
-      <c r="C16" s="39">
-        <v>200000</v>
-      </c>
-      <c r="D16" s="39">
-        <v>200000</v>
-      </c>
-      <c r="E16" s="39">
-        <v>250000</v>
-      </c>
-      <c r="F16" s="39">
-        <v>250000</v>
-      </c>
-      <c r="G16" s="39">
-        <v>250000</v>
-      </c>
-      <c r="H16" s="39"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
-        <v>280</v>
-      </c>
-      <c r="B17" s="39">
-        <v>130000</v>
-      </c>
-      <c r="C17" s="39">
-        <v>130000</v>
-      </c>
-      <c r="D17" s="39">
-        <v>150000</v>
-      </c>
-      <c r="E17" s="39">
-        <v>150000</v>
-      </c>
-      <c r="F17" s="39">
-        <v>150000</v>
-      </c>
-      <c r="G17" s="39">
-        <v>150000</v>
-      </c>
-      <c r="H17" s="39"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
-        <v>280</v>
-      </c>
-      <c r="B18" s="39">
-        <v>130000</v>
-      </c>
-      <c r="C18" s="39">
-        <v>130000</v>
-      </c>
-      <c r="D18" s="39">
-        <v>130000</v>
-      </c>
-      <c r="E18" s="39">
-        <v>150000</v>
-      </c>
-      <c r="F18" s="39">
-        <v>150000</v>
-      </c>
-      <c r="G18" s="39">
-        <v>150000</v>
-      </c>
-      <c r="H18" s="39"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="45" t="s">
-        <v>286</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="B20" s="39">
-        <v>200000</v>
-      </c>
-      <c r="C20" s="39">
-        <v>200000</v>
-      </c>
-      <c r="D20" s="39">
-        <v>200000</v>
-      </c>
-      <c r="E20" s="39">
-        <v>200000</v>
-      </c>
-      <c r="F20" s="39">
-        <v>200000</v>
-      </c>
-      <c r="G20" s="39">
-        <v>200000</v>
-      </c>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="36" t="s">
-        <v>284</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39">
-        <v>100000</v>
-      </c>
-      <c r="E21" s="39">
-        <v>100000</v>
-      </c>
-      <c r="F21" s="39">
-        <v>100000</v>
-      </c>
-      <c r="G21" s="39">
-        <v>100000</v>
-      </c>
-      <c r="H21" s="39"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39">
-        <v>100000</v>
-      </c>
-      <c r="E22" s="39">
-        <v>100000</v>
-      </c>
-      <c r="F22" s="39">
-        <v>100000</v>
-      </c>
-      <c r="G22" s="39">
-        <v>100000</v>
-      </c>
-      <c r="H22" s="39"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="36" t="s">
-        <v>283</v>
-      </c>
-      <c r="B24" s="39">
-        <v>100000</v>
-      </c>
-      <c r="C24" s="39">
-        <v>100000</v>
-      </c>
-      <c r="D24" s="39">
-        <v>100000</v>
-      </c>
-      <c r="E24" s="39">
-        <v>100000</v>
-      </c>
-      <c r="F24" s="39">
-        <v>100000</v>
-      </c>
-      <c r="G24" s="39">
-        <v>100000</v>
-      </c>
-      <c r="H24" s="39"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="36" t="s">
-        <v>284</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39">
-        <v>80000</v>
-      </c>
-      <c r="D25" s="39">
-        <v>80000</v>
-      </c>
-      <c r="E25" s="39">
-        <v>80000</v>
-      </c>
-      <c r="F25" s="39">
-        <v>80000</v>
-      </c>
-      <c r="G25" s="39">
-        <v>80000</v>
-      </c>
-      <c r="H25" s="39"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39">
-        <v>80000</v>
-      </c>
-      <c r="E26" s="39">
-        <v>80000</v>
-      </c>
-      <c r="F26" s="39">
-        <v>80000</v>
-      </c>
-      <c r="G26" s="39">
-        <v>80000</v>
-      </c>
-      <c r="H26" s="39"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="36" t="s">
-        <v>288</v>
-      </c>
-      <c r="B28" s="39">
-        <v>100000</v>
-      </c>
-      <c r="C28" s="39">
-        <v>100000</v>
-      </c>
-      <c r="D28" s="39">
-        <v>100000</v>
-      </c>
-      <c r="E28" s="39">
-        <v>100000</v>
-      </c>
-      <c r="F28" s="39">
-        <v>100000</v>
-      </c>
-      <c r="G28" s="39">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="36" t="s">
-        <v>284</v>
-      </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39">
-        <v>80000</v>
-      </c>
-      <c r="D29" s="39">
-        <v>80000</v>
-      </c>
-      <c r="E29" s="39">
-        <v>80000</v>
-      </c>
-      <c r="F29" s="39">
-        <v>80000</v>
-      </c>
-      <c r="G29" s="39">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39">
-        <v>80000</v>
-      </c>
-      <c r="E30" s="39">
-        <v>80000</v>
-      </c>
-      <c r="F30" s="39">
-        <v>80000</v>
-      </c>
-      <c r="G30" s="39">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="46" t="s">
-        <v>290</v>
-      </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="36" t="s">
-        <v>288</v>
-      </c>
-      <c r="B32" s="39">
-        <v>130000</v>
-      </c>
-      <c r="C32" s="39">
-        <v>130000</v>
-      </c>
-      <c r="D32" s="39">
-        <v>130000</v>
-      </c>
-      <c r="E32" s="39">
-        <v>130000</v>
-      </c>
-      <c r="F32" s="39">
-        <v>130000</v>
-      </c>
-      <c r="G32" s="39">
-        <v>130000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="36"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-    </row>
-    <row r="35" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43" t="s">
-        <v>289</v>
-      </c>
-      <c r="B35" s="44">
-        <f>SUM(B10:B32)</f>
-        <v>1790000</v>
-      </c>
-      <c r="C35" s="44">
-        <f t="shared" ref="C35:G35" si="3">SUM(C10:C32)</f>
-        <v>1950000</v>
-      </c>
-      <c r="D35" s="44">
-        <f t="shared" si="3"/>
-        <v>2780000</v>
-      </c>
-      <c r="E35" s="44">
-        <f t="shared" si="3"/>
-        <v>2900000</v>
-      </c>
-      <c r="F35" s="44">
-        <f t="shared" si="3"/>
-        <v>2900000</v>
-      </c>
-      <c r="G35" s="44">
-        <f t="shared" si="3"/>
-        <v>3200000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="46" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B38" s="39">
-        <f>120000*12</f>
-        <v>1440000</v>
-      </c>
-      <c r="C38" s="39">
-        <f t="shared" ref="C38:G38" si="4">120000*12</f>
-        <v>1440000</v>
-      </c>
-      <c r="D38" s="39">
-        <f t="shared" si="4"/>
-        <v>1440000</v>
-      </c>
-      <c r="E38" s="39">
-        <f t="shared" si="4"/>
-        <v>1440000</v>
-      </c>
-      <c r="F38" s="39">
-        <f t="shared" si="4"/>
-        <v>1440000</v>
-      </c>
-      <c r="G38" s="39">
-        <f t="shared" si="4"/>
-        <v>1440000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="B39" s="39">
-        <v>50000</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="36" t="s">
-        <v>292</v>
-      </c>
-      <c r="B40" s="39">
-        <v>10000</v>
-      </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="36" t="s">
-        <v>293</v>
-      </c>
-      <c r="B41" s="39">
-        <v>10000</v>
-      </c>
-      <c r="C41" s="39">
-        <v>10000</v>
-      </c>
-      <c r="D41" s="39">
-        <v>10000</v>
-      </c>
-      <c r="E41" s="39">
-        <v>10000</v>
-      </c>
-      <c r="F41" s="39">
-        <v>10000</v>
-      </c>
-      <c r="G41" s="39">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="36" t="s">
-        <v>296</v>
-      </c>
-      <c r="B42" s="39">
-        <v>10000</v>
-      </c>
-      <c r="C42" s="39">
-        <v>10000</v>
-      </c>
-      <c r="D42" s="39">
-        <v>10000</v>
-      </c>
-      <c r="E42" s="39">
-        <v>10000</v>
-      </c>
-      <c r="F42" s="39">
-        <v>10000</v>
-      </c>
-      <c r="G42" s="39">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="36" t="s">
-        <v>297</v>
-      </c>
-      <c r="B43" s="39">
-        <v>10000</v>
-      </c>
-      <c r="C43" s="39">
-        <v>10000</v>
-      </c>
-      <c r="D43" s="39">
-        <v>10000</v>
-      </c>
-      <c r="E43" s="39">
-        <v>10000</v>
-      </c>
-      <c r="F43" s="39">
-        <v>10000</v>
-      </c>
-      <c r="G43" s="39">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="36"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="36"/>
+      <c r="B57" s="47">
+        <f>B6-B56</f>
+        <v>-1412000</v>
+      </c>
+      <c r="C57" s="47">
+        <f t="shared" ref="C57:G57" si="10">C6-C56</f>
+        <v>-1852000</v>
+      </c>
+      <c r="D57" s="47">
+        <f t="shared" si="10"/>
+        <v>-2050000</v>
+      </c>
+      <c r="E57" s="47">
+        <f t="shared" si="10"/>
+        <v>-2660000</v>
+      </c>
+      <c r="F57" s="47">
+        <f t="shared" si="10"/>
+        <v>-2330000</v>
+      </c>
+      <c r="G57" s="47">
+        <f t="shared" si="10"/>
+        <v>-2250000</v>
+      </c>
+      <c r="H57" s="47">
+        <f t="shared" ref="H57" si="11">H6-H56</f>
+        <v>-410000</v>
+      </c>
+      <c r="I57" s="47">
+        <f t="shared" ref="I57" si="12">I6-I56</f>
+        <v>4500000</v>
+      </c>
+      <c r="J57" s="47">
+        <f t="shared" ref="J57" si="13">J6-J56</f>
+        <v>14220000</v>
+      </c>
+      <c r="K57" s="47">
+        <f t="shared" ref="K57" si="14">K6-K56</f>
+        <v>33660000</v>
+      </c>
+      <c r="L57" s="47">
+        <f t="shared" ref="L57" si="15">L6-L56</f>
+        <v>72540000</v>
+      </c>
+      <c r="M57" s="47"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15453,10 +16463,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="49"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -15475,10 +16485,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="49"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
updated financials and deck
</commit_message>
<xml_diff>
--- a/Daily Project Journal_V2.xlsx
+++ b/Daily Project Journal_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2FCF7C-A13D-4173-829E-54F59FB8F76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64E438-5A52-468B-8776-29269BD7BF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="1" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="877" activeTab="2" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualESG" sheetId="14" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Monetization" sheetId="5" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -13404,7 +13405,7 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -13648,8 +13649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8991098-D6BF-4772-AB0B-B5195386BBAD}">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -13748,36 +13749,36 @@
         <v>100</v>
       </c>
       <c r="D3" s="40">
-        <f>C3*1.5</f>
-        <v>150</v>
+        <f>C3*2</f>
+        <v>200</v>
       </c>
       <c r="E3" s="40">
-        <f t="shared" ref="E3:G3" si="0">D3*1.5</f>
-        <v>225</v>
+        <f t="shared" ref="E3:H3" si="0">D3*2</f>
+        <v>400</v>
       </c>
       <c r="F3" s="40">
         <f t="shared" si="0"/>
-        <v>337.5</v>
+        <v>800</v>
       </c>
       <c r="G3" s="40">
         <f t="shared" si="0"/>
-        <v>506.25</v>
+        <v>1600</v>
       </c>
       <c r="H3" s="40">
-        <f>G3*2</f>
-        <v>1012.5</v>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="I3" s="40">
-        <f t="shared" ref="I3:L3" si="1">H3*2</f>
-        <v>2025</v>
+        <f>H3*1.5</f>
+        <v>4800</v>
       </c>
       <c r="J3" s="40">
-        <f t="shared" si="1"/>
-        <v>4050</v>
+        <f t="shared" ref="J3:L3" si="1">I3*1.5</f>
+        <v>7200</v>
       </c>
       <c r="K3" s="40">
         <f t="shared" si="1"/>
-        <v>8100</v>
+        <v>10800</v>
       </c>
       <c r="L3" s="40">
         <f t="shared" si="1"/>
@@ -13792,7 +13793,7 @@
         <v>261</v>
       </c>
       <c r="P3" s="42">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -13837,7 +13838,7 @@
       </c>
       <c r="P4" s="38">
         <f>P3*SUM(P1:P2)</f>
-        <v>12600</v>
+        <v>63000</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -13889,35 +13890,35 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" si="2"/>
-        <v>540000</v>
+        <v>720000</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" si="2"/>
-        <v>810000</v>
+        <v>1440000</v>
       </c>
       <c r="F6" s="43">
         <f t="shared" si="2"/>
-        <v>1620000</v>
+        <v>3840000</v>
       </c>
       <c r="G6" s="43">
         <f t="shared" si="2"/>
-        <v>2430000</v>
+        <v>7680000</v>
       </c>
       <c r="H6" s="43">
         <f t="shared" ref="H6:L6" si="3">H3*H4*H5</f>
-        <v>4860000</v>
+        <v>15360000</v>
       </c>
       <c r="I6" s="43">
         <f t="shared" si="3"/>
-        <v>9720000</v>
+        <v>23040000</v>
       </c>
       <c r="J6" s="43">
         <f t="shared" si="3"/>
-        <v>19440000</v>
+        <v>34560000</v>
       </c>
       <c r="K6" s="43">
         <f t="shared" si="3"/>
-        <v>38880000</v>
+        <v>51840000</v>
       </c>
       <c r="L6" s="43">
         <f t="shared" si="3"/>
@@ -15411,35 +15412,35 @@
       </c>
       <c r="D57" s="47">
         <f t="shared" si="10"/>
-        <v>-2050000</v>
+        <v>-1870000</v>
       </c>
       <c r="E57" s="47">
         <f t="shared" si="10"/>
-        <v>-2660000</v>
+        <v>-2030000</v>
       </c>
       <c r="F57" s="47">
         <f t="shared" si="10"/>
-        <v>-2330000</v>
+        <v>-110000</v>
       </c>
       <c r="G57" s="47">
         <f t="shared" si="10"/>
-        <v>-2250000</v>
+        <v>3000000</v>
       </c>
       <c r="H57" s="47">
         <f t="shared" ref="H57" si="11">H6-H56</f>
-        <v>-410000</v>
+        <v>10090000</v>
       </c>
       <c r="I57" s="47">
         <f t="shared" ref="I57" si="12">I6-I56</f>
-        <v>4500000</v>
+        <v>17820000</v>
       </c>
       <c r="J57" s="47">
         <f t="shared" ref="J57" si="13">J6-J56</f>
-        <v>14220000</v>
+        <v>29340000</v>
       </c>
       <c r="K57" s="47">
         <f t="shared" ref="K57" si="14">K6-K56</f>
-        <v>33660000</v>
+        <v>46620000</v>
       </c>
       <c r="L57" s="47">
         <f t="shared" ref="L57" si="15">L6-L56</f>

</xml_diff>

<commit_message>
updated for individual sustainability
</commit_message>
<xml_diff>
--- a/Daily Project Journal_V2.xlsx
+++ b/Daily Project Journal_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchung\Personal\LearnH2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\LearnH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF93C62-E14A-4A7C-BCD3-1350303F9FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1877573-EE86-4BF8-B7D8-9027575BCD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="8170" tabRatio="877" xr2:uid="{0B88B0BF-69A4-467A-8E1E-488C50FA036B}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualESG" sheetId="14" r:id="rId1"/>
@@ -1493,14 +1493,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2072,16 +2072,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>549088</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>121210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241113</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4296</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2096,8 +2096,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2755900" y="2339975"/>
-          <a:ext cx="911225" cy="450850"/>
+          <a:off x="2386853" y="121210"/>
+          <a:ext cx="917201" cy="443380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3884,6 +3884,74 @@
               </a:solidFill>
             </a:rPr>
             <a:t>Tax returns</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>321234</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>97119</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>159496</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC926854-6981-4D78-AAB8-8C1EDA41F48A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771587" y="2330822"/>
+          <a:ext cx="1001061" cy="443380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>car insurance or carfax</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -13872,161 +13940,161 @@
   </sheetPr>
   <dimension ref="A23:C61"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AC1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="25" max="29" width="9.7109375" customWidth="1"/>
+    <col min="25" max="29" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="55"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="56" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="57" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C29" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C30" s="32" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C32" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" s="33" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" s="33" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" s="33" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" s="1"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" s="1" t="s">
         <v>183</v>
       </c>
@@ -14045,7 +14113,7 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14060,9 +14128,9 @@
       <selection activeCell="B7" sqref="B7:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -14070,7 +14138,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -14078,7 +14146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -14100,17 +14168,17 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="6" max="9" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" customWidth="1"/>
+    <col min="6" max="9" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>136</v>
       </c>
@@ -14133,7 +14201,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -14149,7 +14217,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="31"/>
     </row>
-    <row r="3" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -14161,7 +14229,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="31"/>
     </row>
-    <row r="4" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -14173,7 +14241,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="31"/>
     </row>
-    <row r="5" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -14185,7 +14253,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="31"/>
     </row>
-    <row r="6" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -14203,7 +14271,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -14215,7 +14283,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="31"/>
     </row>
-    <row r="8" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -14238,7 +14306,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -14261,7 +14329,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -14284,7 +14352,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -14303,7 +14371,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -14340,24 +14408,24 @@
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
@@ -14376,19 +14444,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -14406,49 +14474,49 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -14466,42 +14534,42 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -14516,25 +14584,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905ACA74-69C8-478A-9F42-EDAA083897E5}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="5" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="3" max="5" width="39.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="55" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C1" s="59" t="s">
         <v>309</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>329</v>
       </c>
@@ -14548,97 +14616,97 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>308</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="58" t="s">
         <v>316</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="58" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>310</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="58" t="s">
         <v>319</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="58" t="s">
         <v>320</v>
       </c>
-      <c r="E4" s="59"/>
-    </row>
-    <row r="5" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="58"/>
+    </row>
+    <row r="5" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="58" t="s">
         <v>322</v>
       </c>
-      <c r="E5" s="59"/>
-    </row>
-    <row r="6" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="58"/>
+    </row>
+    <row r="6" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>312</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>323</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="58" t="s">
         <v>324</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="58" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>313</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="58" t="s">
         <v>326</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="58" t="s">
         <v>327</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="58" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>314</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="58" t="s">
         <v>330</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="58" t="s">
         <v>331</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="58" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>315</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="58" t="s">
         <v>333</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="58" t="s">
         <v>334</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="58" t="s">
         <v>335</v>
       </c>
     </row>
@@ -14657,19 +14725,19 @@
   </sheetPr>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="103.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="103.1796875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -14677,7 +14745,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>131</v>
       </c>
@@ -14685,37 +14753,37 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>132</v>
       </c>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>293</v>
       </c>
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>284</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>286</v>
       </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>287</v>
       </c>
@@ -14723,37 +14791,37 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>288</v>
       </c>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>289</v>
       </c>
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>294</v>
       </c>
       <c r="B11" s="9"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>3</v>
       </c>
@@ -14761,19 +14829,19 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>95</v>
       </c>
@@ -14781,19 +14849,19 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B20" s="17"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>89</v>
       </c>
@@ -14801,19 +14869,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B22" s="19"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B23" s="19"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>76</v>
       </c>
@@ -14821,86 +14889,86 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
     </row>
-    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>84</v>
       </c>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="14" t="s">
         <v>77</v>
       </c>
@@ -14920,20 +14988,20 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="35" customWidth="1"/>
-    <col min="5" max="12" width="15.5703125" style="35"/>
-    <col min="13" max="13" width="3.140625" style="35" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="35"/>
-    <col min="15" max="15" width="24.85546875" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="15.5703125" style="35"/>
+    <col min="1" max="1" width="25.81640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" style="35" customWidth="1"/>
+    <col min="5" max="12" width="15.54296875" style="35"/>
+    <col min="13" max="13" width="3.1796875" style="35" customWidth="1"/>
+    <col min="14" max="14" width="15.54296875" style="35"/>
+    <col min="15" max="15" width="24.81640625" style="35" customWidth="1"/>
+    <col min="16" max="16384" width="15.54296875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>295</v>
       </c>
@@ -14981,7 +15049,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="39" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="39" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
         <v>296</v>
       </c>
@@ -15013,7 +15081,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="39" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="39" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="39" t="s">
         <v>301</v>
       </c>
@@ -15034,7 +15102,7 @@
       </c>
       <c r="P3" s="40"/>
     </row>
-    <row r="4" spans="1:16" s="39" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="39" customFormat="1" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="39" t="s">
         <v>297</v>
       </c>
@@ -15046,16 +15114,16 @@
       </c>
       <c r="P4" s="40"/>
     </row>
-    <row r="5" spans="1:16" s="39" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="39" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P5" s="40"/>
     </row>
-    <row r="6" spans="1:16" s="39" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="39" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P6" s="40"/>
     </row>
-    <row r="7" spans="1:16" s="39" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="39" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P7" s="40"/>
     </row>
-    <row r="8" spans="1:16" s="39" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="39" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="39" t="s">
         <v>218</v>
       </c>
@@ -15111,7 +15179,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>219</v>
       </c>
@@ -15156,7 +15224,7 @@
         <v>12600</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>220</v>
       </c>
@@ -15194,7 +15262,7 @@
       <c r="M10" s="38"/>
       <c r="N10" s="38"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>215</v>
       </c>
@@ -15242,12 +15310,12 @@
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="44" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
         <v>223</v>
       </c>
@@ -15286,7 +15354,7 @@
       </c>
       <c r="M15" s="43"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>225</v>
       </c>
@@ -15325,7 +15393,7 @@
       </c>
       <c r="M16" s="43"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>224</v>
       </c>
@@ -15364,7 +15432,7 @@
       </c>
       <c r="M17" s="43"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
         <v>227</v>
       </c>
@@ -15382,7 +15450,7 @@
       <c r="M18" s="43"/>
       <c r="N18" s="43"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="35" t="s">
         <v>243</v>
       </c>
@@ -15422,7 +15490,7 @@
       <c r="M19" s="43"/>
       <c r="N19" s="43"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="35" t="s">
         <v>228</v>
       </c>
@@ -15462,7 +15530,7 @@
       <c r="M20" s="43"/>
       <c r="N20" s="43"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
         <v>228</v>
       </c>
@@ -15496,7 +15564,7 @@
       <c r="M21" s="43"/>
       <c r="N21" s="43"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>229</v>
       </c>
@@ -15536,7 +15604,7 @@
       <c r="M22" s="43"/>
       <c r="N22" s="43"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="35" t="s">
         <v>229</v>
       </c>
@@ -15570,7 +15638,7 @@
       <c r="M23" s="43"/>
       <c r="N23" s="43"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
         <v>259</v>
       </c>
@@ -15604,7 +15672,7 @@
       <c r="M24" s="43"/>
       <c r="N24" s="43"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>228</v>
       </c>
@@ -15638,7 +15706,7 @@
       <c r="M25" s="43"/>
       <c r="N25" s="43"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
         <v>229</v>
       </c>
@@ -15672,7 +15740,7 @@
       <c r="M26" s="43"/>
       <c r="N26" s="43"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
         <v>229</v>
       </c>
@@ -15706,7 +15774,7 @@
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="44" t="s">
         <v>235</v>
       </c>
@@ -15724,7 +15792,7 @@
       <c r="M28" s="43"/>
       <c r="N28" s="43"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="35" t="s">
         <v>236</v>
       </c>
@@ -15760,7 +15828,7 @@
       <c r="M29" s="43"/>
       <c r="N29" s="43"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="35" t="s">
         <v>233</v>
       </c>
@@ -15790,7 +15858,7 @@
       <c r="M30" s="43"/>
       <c r="N30" s="43"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>234</v>
       </c>
@@ -15820,7 +15888,7 @@
       <c r="M31" s="43"/>
       <c r="N31" s="43"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>260</v>
       </c>
@@ -15838,7 +15906,7 @@
       <c r="M32" s="43"/>
       <c r="N32" s="43"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>261</v>
       </c>
@@ -15856,7 +15924,7 @@
       <c r="M33" s="43"/>
       <c r="N33" s="43"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="44" t="s">
         <v>230</v>
       </c>
@@ -15874,7 +15942,7 @@
       <c r="M34" s="43"/>
       <c r="N34" s="43"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>232</v>
       </c>
@@ -15914,7 +15982,7 @@
       <c r="M35" s="43"/>
       <c r="N35" s="43"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>233</v>
       </c>
@@ -15952,7 +16020,7 @@
       <c r="M36" s="43"/>
       <c r="N36" s="43"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>234</v>
       </c>
@@ -15988,7 +16056,7 @@
       <c r="M37" s="43"/>
       <c r="N37" s="43"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
         <v>260</v>
       </c>
@@ -16018,7 +16086,7 @@
       <c r="M38" s="43"/>
       <c r="N38" s="43"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>261</v>
       </c>
@@ -16048,7 +16116,7 @@
       <c r="M39" s="43"/>
       <c r="N39" s="43"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="44" t="s">
         <v>231</v>
       </c>
@@ -16066,7 +16134,7 @@
       <c r="M40" s="43"/>
       <c r="N40" s="43"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="35" t="s">
         <v>237</v>
       </c>
@@ -16101,7 +16169,7 @@
       </c>
       <c r="M41" s="43"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>233</v>
       </c>
@@ -16136,7 +16204,7 @@
       </c>
       <c r="M42" s="43"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="35" t="s">
         <v>234</v>
       </c>
@@ -16171,7 +16239,7 @@
       </c>
       <c r="M43" s="43"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="45" t="s">
         <v>239</v>
       </c>
@@ -16188,7 +16256,7 @@
       <c r="L44" s="43"/>
       <c r="M44" s="43"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
         <v>237</v>
       </c>
@@ -16223,7 +16291,7 @@
       </c>
       <c r="M45" s="43"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="45" t="s">
         <v>291</v>
       </c>
@@ -16240,7 +16308,7 @@
       <c r="L46" s="43"/>
       <c r="M46" s="43"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>292</v>
       </c>
@@ -16279,7 +16347,7 @@
       </c>
       <c r="M47" s="43"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="45"/>
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
@@ -16294,7 +16362,7 @@
       <c r="L48" s="43"/>
       <c r="M48" s="43"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="45"/>
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -16309,7 +16377,7 @@
       <c r="L49" s="43"/>
       <c r="M49" s="43"/>
     </row>
-    <row r="50" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="46" t="s">
         <v>238</v>
       </c>
@@ -16359,12 +16427,12 @@
       </c>
       <c r="M50" s="47"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="45" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>241</v>
       </c>
@@ -16414,7 +16482,7 @@
       </c>
       <c r="M53" s="43"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>242</v>
       </c>
@@ -16437,7 +16505,7 @@
       <c r="L54" s="43"/>
       <c r="M54" s="43"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="35" t="s">
         <v>240</v>
       </c>
@@ -16460,7 +16528,7 @@
       <c r="L55" s="43"/>
       <c r="M55" s="43"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="35" t="s">
         <v>245</v>
       </c>
@@ -16499,7 +16567,7 @@
       </c>
       <c r="M56" s="43"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="35" t="s">
         <v>246</v>
       </c>
@@ -16538,7 +16606,7 @@
       </c>
       <c r="M57" s="43"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="35" t="s">
         <v>247</v>
       </c>
@@ -16577,7 +16645,7 @@
       </c>
       <c r="M58" s="43"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>248</v>
       </c>
@@ -16616,7 +16684,7 @@
       </c>
       <c r="M59" s="43"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="35" t="s">
         <v>249</v>
       </c>
@@ -16666,7 +16734,7 @@
       </c>
       <c r="M61" s="48"/>
     </row>
-    <row r="63" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="46" t="s">
         <v>262</v>
       </c>
@@ -16716,7 +16784,7 @@
       </c>
       <c r="M63" s="47"/>
     </row>
-    <row r="64" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
         <v>252</v>
       </c>
@@ -16783,17 +16851,17 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.54296875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -16816,7 +16884,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45202</v>
       </c>
@@ -16828,7 +16896,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>45152</v>
       </c>
@@ -16840,7 +16908,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -16852,7 +16920,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>45144</v>
       </c>
@@ -16864,7 +16932,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>45143</v>
       </c>
@@ -16876,7 +16944,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>45142</v>
       </c>
@@ -16888,7 +16956,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>45141</v>
       </c>
@@ -16900,7 +16968,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>45140</v>
       </c>
@@ -16912,7 +16980,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>45140</v>
       </c>
@@ -16924,7 +16992,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>45139</v>
       </c>
@@ -16936,7 +17004,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>45138</v>
       </c>
@@ -16948,7 +17016,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>45137</v>
       </c>
@@ -16960,7 +17028,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>45136</v>
       </c>
@@ -16972,7 +17040,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>45135</v>
       </c>
@@ -16984,7 +17052,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="22">
         <v>45134</v>
       </c>
@@ -16996,7 +17064,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>45133</v>
       </c>
@@ -17008,7 +17076,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>45132</v>
       </c>
@@ -17020,7 +17088,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>45131</v>
       </c>
@@ -17032,7 +17100,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>45130</v>
       </c>
@@ -17044,7 +17112,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>45129</v>
       </c>
@@ -17056,7 +17124,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>45128</v>
       </c>
@@ -17068,7 +17136,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>45127</v>
       </c>
@@ -17080,7 +17148,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>45126</v>
       </c>
@@ -17092,7 +17160,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>45125</v>
       </c>
@@ -17104,7 +17172,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>45124</v>
       </c>
@@ -17116,7 +17184,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>45123</v>
       </c>
@@ -17128,7 +17196,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>45122</v>
       </c>
@@ -17140,7 +17208,7 @@
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>45121</v>
       </c>
@@ -17152,7 +17220,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>45120</v>
       </c>
@@ -17164,7 +17232,7 @@
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>45119</v>
       </c>
@@ -17176,7 +17244,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>45118</v>
       </c>
@@ -17188,7 +17256,7 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>45117</v>
       </c>
@@ -17200,7 +17268,7 @@
       </c>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>45116</v>
       </c>
@@ -17212,7 +17280,7 @@
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>45115</v>
       </c>
@@ -17224,7 +17292,7 @@
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>45114</v>
       </c>
@@ -17236,7 +17304,7 @@
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>45113</v>
       </c>
@@ -17248,7 +17316,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>45112</v>
       </c>
@@ -17260,7 +17328,7 @@
       </c>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>45111</v>
       </c>
@@ -17272,7 +17340,7 @@
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>45110</v>
       </c>
@@ -17284,7 +17352,7 @@
       </c>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>45109</v>
       </c>
@@ -17296,7 +17364,7 @@
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>45108</v>
       </c>
@@ -17308,7 +17376,7 @@
       </c>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>45107</v>
       </c>
@@ -17318,7 +17386,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>45106</v>
       </c>
@@ -17330,7 +17398,7 @@
       </c>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>45105</v>
       </c>
@@ -17344,7 +17412,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>45104</v>
       </c>
@@ -17356,7 +17424,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>45103</v>
       </c>
@@ -17367,7 +17435,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>45102</v>
       </c>
@@ -17381,7 +17449,7 @@
         <v>45110</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>45102</v>
       </c>
@@ -17395,7 +17463,7 @@
         <v>45117</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>45101</v>
       </c>
@@ -17406,7 +17474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>45101</v>
       </c>
@@ -17419,7 +17487,7 @@
       <c r="D51" s="9"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
         <v>45101</v>
       </c>
@@ -17431,7 +17499,7 @@
       </c>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>45101</v>
       </c>
@@ -17443,7 +17511,7 @@
       </c>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>45100</v>
       </c>
@@ -17454,7 +17522,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>45100</v>
       </c>
@@ -17465,7 +17533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>45100</v>
       </c>
@@ -17476,7 +17544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>45100</v>
       </c>
@@ -17487,7 +17555,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>45100</v>
       </c>
@@ -17498,7 +17566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>45100</v>
       </c>
@@ -17509,7 +17577,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>45099</v>
       </c>
@@ -17520,7 +17588,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>45099</v>
       </c>
@@ -17558,14 +17626,14 @@
       <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" customWidth="1"/>
+    <col min="3" max="3" width="55.453125" customWidth="1"/>
+    <col min="4" max="4" width="53.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>267</v>
       </c>
@@ -17579,7 +17647,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
         <v>270</v>
       </c>
@@ -17593,7 +17661,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="49" t="s">
         <v>271</v>
       </c>
@@ -17607,34 +17675,34 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="49"/>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
       <c r="D4" s="49"/>
     </row>
-    <row r="5" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="49"/>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
     </row>
-    <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="49"/>
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
     </row>
-    <row r="8" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
     </row>
-    <row r="9" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C9" s="49"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="49" t="s">
         <v>276</v>
       </c>
@@ -17648,7 +17716,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="49" t="s">
         <v>279</v>
       </c>
@@ -17658,7 +17726,7 @@
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="49" t="s">
         <v>279</v>
       </c>
@@ -17668,7 +17736,7 @@
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="49" t="s">
         <v>279</v>
       </c>
@@ -17678,85 +17746,85 @@
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
       <c r="D14" s="50"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="50"/>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
       <c r="D15" s="50"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="50"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="50"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="50"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="50"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="50"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="50"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="50"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="50"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="50"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="50"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="50"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="50"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="50"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="50"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="50"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="50"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="50"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="50"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="50"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="50"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="50"/>
     </row>
   </sheetData>
@@ -17772,19 +17840,19 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="55"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="59"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -17792,7 +17860,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -17800,13 +17868,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="55"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="59"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -17814,7 +17882,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -17822,7 +17890,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -17830,7 +17898,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -17838,7 +17906,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -17846,7 +17914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -17872,9 +17940,9 @@
       <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -17895,7 +17963,7 @@
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -17916,7 +17984,7 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -17937,7 +18005,7 @@
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -17958,7 +18026,7 @@
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -17979,7 +18047,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -18000,7 +18068,7 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -18021,7 +18089,7 @@
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -18042,7 +18110,7 @@
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -18063,7 +18131,7 @@
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -18084,7 +18152,7 @@
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -18105,7 +18173,7 @@
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -18126,7 +18194,7 @@
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -18147,7 +18215,7 @@
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -18168,7 +18236,7 @@
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -18189,7 +18257,7 @@
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -18210,7 +18278,7 @@
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -18231,7 +18299,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -18252,7 +18320,7 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -18273,7 +18341,7 @@
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -18294,7 +18362,7 @@
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -18315,7 +18383,7 @@
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -18336,7 +18404,7 @@
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -18357,7 +18425,7 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -18378,7 +18446,7 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -18399,7 +18467,7 @@
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -18420,7 +18488,7 @@
       <c r="R26" s="12"/>
       <c r="S26" s="12"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -18441,7 +18509,7 @@
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -18462,7 +18530,7 @@
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -18483,7 +18551,7 @@
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -18504,7 +18572,7 @@
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -18525,7 +18593,7 @@
       <c r="R31" s="12"/>
       <c r="S31" s="12"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -18546,7 +18614,7 @@
       <c r="R32" s="12"/>
       <c r="S32" s="12"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -18567,7 +18635,7 @@
       <c r="R33" s="12"/>
       <c r="S33" s="12"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -18588,7 +18656,7 @@
       <c r="R34" s="12"/>
       <c r="S34" s="12"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -18609,7 +18677,7 @@
       <c r="R35" s="12"/>
       <c r="S35" s="12"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -18630,7 +18698,7 @@
       <c r="R36" s="12"/>
       <c r="S36" s="12"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -18651,7 +18719,7 @@
       <c r="R37" s="20"/>
       <c r="S37" s="20"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -18672,7 +18740,7 @@
       <c r="R38" s="20"/>
       <c r="S38" s="20"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -18693,7 +18761,7 @@
       <c r="R39" s="20"/>
       <c r="S39" s="20"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -18714,7 +18782,7 @@
       <c r="R40" s="20"/>
       <c r="S40" s="20"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
@@ -18735,7 +18803,7 @@
       <c r="R41" s="20"/>
       <c r="S41" s="20"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
@@ -18756,7 +18824,7 @@
       <c r="R42" s="20"/>
       <c r="S42" s="20"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -18777,7 +18845,7 @@
       <c r="R43" s="20"/>
       <c r="S43" s="20"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="20"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -18798,7 +18866,7 @@
       <c r="R44" s="20"/>
       <c r="S44" s="20"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="20"/>
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
@@ -18819,7 +18887,7 @@
       <c r="R45" s="20"/>
       <c r="S45" s="20"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="20"/>
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
@@ -18840,7 +18908,7 @@
       <c r="R46" s="20"/>
       <c r="S46" s="20"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="20"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
@@ -18861,7 +18929,7 @@
       <c r="R47" s="20"/>
       <c r="S47" s="20"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="20"/>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
@@ -18882,7 +18950,7 @@
       <c r="R48" s="20"/>
       <c r="S48" s="20"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
@@ -18903,7 +18971,7 @@
       <c r="R49" s="20"/>
       <c r="S49" s="20"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
@@ -18924,7 +18992,7 @@
       <c r="R50" s="20"/>
       <c r="S50" s="20"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="20"/>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
@@ -18945,7 +19013,7 @@
       <c r="R51" s="20"/>
       <c r="S51" s="20"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="20"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
@@ -18966,7 +19034,7 @@
       <c r="R52" s="20"/>
       <c r="S52" s="20"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
@@ -18987,7 +19055,7 @@
       <c r="R53" s="20"/>
       <c r="S53" s="20"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
@@ -19008,7 +19076,7 @@
       <c r="R54" s="20"/>
       <c r="S54" s="20"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
@@ -19029,7 +19097,7 @@
       <c r="R55" s="20"/>
       <c r="S55" s="20"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
@@ -19050,7 +19118,7 @@
       <c r="R56" s="20"/>
       <c r="S56" s="20"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
@@ -19071,7 +19139,7 @@
       <c r="R57" s="20"/>
       <c r="S57" s="20"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
@@ -19092,7 +19160,7 @@
       <c r="R58" s="20"/>
       <c r="S58" s="20"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
@@ -19127,9 +19195,9 @@
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -19159,7 +19227,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -19187,7 +19255,7 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -19215,7 +19283,7 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -19243,7 +19311,7 @@
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -19271,7 +19339,7 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -19299,7 +19367,7 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
     </row>
-    <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -19327,7 +19395,7 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -19355,7 +19423,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -19383,7 +19451,7 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -19411,7 +19479,7 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
     </row>
-    <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -19439,7 +19507,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
     </row>
-    <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -19467,7 +19535,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -19495,7 +19563,7 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
     </row>
-    <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -19523,7 +19591,7 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
     </row>
-    <row r="15" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -19551,7 +19619,7 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -19579,7 +19647,7 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
     </row>
-    <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -19607,7 +19675,7 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
     </row>
-    <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -19635,7 +19703,7 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
     </row>
-    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -19663,7 +19731,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -19691,7 +19759,7 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
     </row>
-    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -19719,7 +19787,7 @@
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
     </row>
-    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -19747,7 +19815,7 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
     </row>
-    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -19775,7 +19843,7 @@
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -19803,7 +19871,7 @@
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -19831,7 +19899,7 @@
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -19859,7 +19927,7 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -19887,7 +19955,7 @@
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -19915,7 +19983,7 @@
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -19943,7 +20011,7 @@
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -19971,7 +20039,7 @@
       <c r="Y30" s="12"/>
       <c r="Z30" s="12"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -19999,7 +20067,7 @@
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -20027,7 +20095,7 @@
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -20055,7 +20123,7 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -20083,7 +20151,7 @@
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -20111,7 +20179,7 @@
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -20139,7 +20207,7 @@
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -20167,7 +20235,7 @@
       <c r="Y37" s="12"/>
       <c r="Z37" s="12"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -20195,7 +20263,7 @@
       <c r="Y38" s="12"/>
       <c r="Z38" s="12"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -20223,7 +20291,7 @@
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -20251,7 +20319,7 @@
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -20279,7 +20347,7 @@
       <c r="Y41" s="12"/>
       <c r="Z41" s="12"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -20307,7 +20375,7 @@
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -20335,7 +20403,7 @@
       <c r="Y43" s="12"/>
       <c r="Z43" s="12"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -20363,7 +20431,7 @@
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -20391,7 +20459,7 @@
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -20419,7 +20487,7 @@
       <c r="Y46" s="12"/>
       <c r="Z46" s="12"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -20447,7 +20515,7 @@
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -20475,7 +20543,7 @@
       <c r="Y48" s="12"/>
       <c r="Z48" s="12"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -20503,7 +20571,7 @@
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -20531,7 +20599,7 @@
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -20559,7 +20627,7 @@
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -20587,7 +20655,7 @@
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -20615,7 +20683,7 @@
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
@@ -20643,7 +20711,7 @@
       <c r="Y54" s="12"/>
       <c r="Z54" s="12"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -20671,7 +20739,7 @@
       <c r="Y55" s="12"/>
       <c r="Z55" s="12"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -20699,7 +20767,7 @@
       <c r="Y56" s="12"/>
       <c r="Z56" s="12"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
@@ -20727,7 +20795,7 @@
       <c r="Y57" s="12"/>
       <c r="Z57" s="12"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="12"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -20755,7 +20823,7 @@
       <c r="Y58" s="12"/>
       <c r="Z58" s="12"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="12"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -20783,7 +20851,7 @@
       <c r="Y59" s="12"/>
       <c r="Z59" s="12"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="12"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
@@ -20811,7 +20879,7 @@
       <c r="Y60" s="12"/>
       <c r="Z60" s="12"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="12"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
@@ -20839,7 +20907,7 @@
       <c r="Y61" s="12"/>
       <c r="Z61" s="12"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="12"/>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
@@ -20867,7 +20935,7 @@
       <c r="Y62" s="12"/>
       <c r="Z62" s="12"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="12"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -20895,7 +20963,7 @@
       <c r="Y63" s="12"/>
       <c r="Z63" s="12"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="12"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
@@ -20923,7 +20991,7 @@
       <c r="Y64" s="12"/>
       <c r="Z64" s="12"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="12"/>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
@@ -20951,7 +21019,7 @@
       <c r="Y65" s="12"/>
       <c r="Z65" s="12"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -20979,7 +21047,7 @@
       <c r="Y66" s="12"/>
       <c r="Z66" s="12"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="12"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
@@ -21007,7 +21075,7 @@
       <c r="Y67" s="12"/>
       <c r="Z67" s="12"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="12"/>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
@@ -21035,7 +21103,7 @@
       <c r="Y68" s="12"/>
       <c r="Z68" s="12"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="12"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
@@ -21063,7 +21131,7 @@
       <c r="Y69" s="12"/>
       <c r="Z69" s="12"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="12"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
@@ -21091,7 +21159,7 @@
       <c r="Y70" s="12"/>
       <c r="Z70" s="12"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="12"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>

</xml_diff>